<commit_message>
allow player to move in 4 directions
</commit_message>
<xml_diff>
--- a/component/message.xlsx
+++ b/component/message.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmh98\Desktop\component\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmh98\Desktop\finalproject-seattle-group\component\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544EA45F-EC72-4C90-9A36-36A052511ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{253E76D5-4DF9-4D0D-B363-5BF493D4AA2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>message1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,6 +95,10 @@
   </si>
   <si>
     <t>position of y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>button press 1 = up / -1 = down;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -423,7 +427,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A7" sqref="A7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -451,44 +455,76 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B2">
-        <v>123</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B4">
+        <v>111</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B3">
+      <c r="B5">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
         <v>124</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>101</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="b">
+      <c r="E8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>102</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
         <v>17</v>
       </c>
     </row>
@@ -497,7 +533,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -511,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B16">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -525,7 +561,7 @@
         <v>13</v>
       </c>
       <c r="B17">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>

</xml_diff>